<commit_message>
Added checks for birth before death and divorce after marriage. Added corresponding unit tests. Fixed error where one list is shared across multiple objects, which caused childrens to be added to multiple families.
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunaksaklikar/Documents/cs555/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Project\SSW555\CS555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB461B-9CCF-4C49-8E99-352189523D73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3CF031-79A8-43E4-8B89-45DAD5C93177}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1013,7 +1013,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42796</c:v>
@@ -1075,7 +1075,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2056,16 +2056,16 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2197,16 +2197,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2223,10 +2223,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
     </row>
   </sheetData>
@@ -2244,48 +2244,48 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -2425,17 +2425,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40442</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40455</v>
       </c>
@@ -2500,23 +2500,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="33.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
     <col min="9" max="9" width="20" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2604,8 +2604,17 @@
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6">
+        <v>42801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2624,8 +2633,14 @@
       <c r="F5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G5">
+        <v>130</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2645,7 +2660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2665,7 +2680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2685,7 +2700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2705,7 +2720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2725,7 +2740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2745,21 +2760,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -2779,9 +2794,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2825,9 +2840,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2870,9 +2885,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2911,17 +2926,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -2932,7 +2947,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -2943,7 +2958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -2954,7 +2969,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2965,7 +2980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -2976,7 +2991,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2987,7 +3002,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -2998,7 +3013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3009,7 +3024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3020,7 +3035,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3031,7 +3046,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3042,7 +3057,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3053,7 +3068,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3064,7 +3079,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3075,7 +3090,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3086,7 +3101,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3097,7 +3112,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3108,7 +3123,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3119,7 +3134,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3130,7 +3145,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3141,7 +3156,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3152,7 +3167,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3163,7 +3178,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3174,7 +3189,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3185,7 +3200,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3196,7 +3211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3207,7 +3222,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3218,7 +3233,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3229,7 +3244,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3240,7 +3255,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3251,7 +3266,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3262,7 +3277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3273,7 +3288,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3284,7 +3299,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3295,7 +3310,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3306,7 +3321,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3317,7 +3332,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3328,7 +3343,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3339,7 +3354,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3350,7 +3365,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3361,7 +3376,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3372,7 +3387,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3383,7 +3398,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Added SQLite database. Made it easier to add new validation functions to objects.
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Project\SSW555\CS555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3CF031-79A8-43E4-8B89-45DAD5C93177}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426A678-2C3D-46DC-9D5A-D1DD7DDFCA75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2501,7 +2501,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2718,6 +2718,15 @@
       </c>
       <c r="F9">
         <v>2</v>
+      </c>
+      <c r="G9">
+        <v>180</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6">
+        <v>42803</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2927,7 +2936,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>